<commit_message>
improvement: add instruction video
</commit_message>
<xml_diff>
--- a/data/dummyData.xlsx
+++ b/data/dummyData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c500a9faf79b22a/Desktop/newTest2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c500a9faf79b22a/Documents/Projects/projects/complete/FLDLGenerator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{98C24981-2791-4BE0-B286-8B650027356D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2802463-19A2-4361-9636-F1F78904B2CF}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{98C24981-2791-4BE0-B286-8B650027356D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C4CB3C3-A51A-47BC-A5C4-64CE6A34A929}"/>
   <bookViews>
-    <workbookView xWindow="4147" yWindow="2295" windowWidth="16200" windowHeight="9983" xr2:uid="{7399256E-38A8-479F-9C73-5FEBCBF0C5BC}"/>
+    <workbookView minimized="1" xWindow="4147" yWindow="2295" windowWidth="16200" windowHeight="9983" xr2:uid="{7399256E-38A8-479F-9C73-5FEBCBF0C5BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Profiles" sheetId="1" r:id="rId1"/>
@@ -168,8 +168,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -197,14 +205,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -215,6 +254,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAAF5284-5BA5-4CEC-B896-4BBAB61E3460}" name="Table1" displayName="Table1" ref="A1:J10" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:J10" xr:uid="{EAAF5284-5BA5-4CEC-B896-4BBAB61E3460}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{88ED6355-1C6C-4C46-BE54-3B508F77C133}" name="firstName"/>
+    <tableColumn id="2" xr3:uid="{E9C9C040-273C-4127-9FE4-7009F2D8AFED}" name="lastName"/>
+    <tableColumn id="3" xr3:uid="{8A106F75-4AC8-48CA-81D4-51DDE9423656}" name="Gender"/>
+    <tableColumn id="4" xr3:uid="{EB90DA44-B51F-4F0A-9AB3-9DF417D32E7A}" name="Country"/>
+    <tableColumn id="5" xr3:uid="{8BE95EA1-3663-42C5-9BFD-8DD1D49735A6}" name="Age"/>
+    <tableColumn id="6" xr3:uid="{B78F0898-A08A-404E-9E5C-A6A98410843A}" name="Month" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{1F1788FB-044A-4D6F-B7BC-D6CFBC6B2FD0}" name="Day" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{3B2D02B5-2833-4B1D-9531-B85B96152C05}" name="Year" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{BB0B4859-B433-46F6-85C7-C68F15A4F62A}" name="Date"/>
+    <tableColumn id="10" xr3:uid="{348FBEBE-255C-4D8A-B3BE-6C425B60CAA7}" name="Id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -516,44 +574,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8DE960-7499-48B1-AC9C-CC1B67239306}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="8" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.73046875" customWidth="1"/>
+    <col min="6" max="6" width="8.1328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.19921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -848,6 +915,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>